<commit_message>
Merged Mendix Test Plan updated for Create Vendor for JDE
TestCase and TestData to be merged to make work the Setting Request id
and Global id as per the test Case Name.

Merged JDE scripts for vendor fixes provided for data input removed loop
for selecting value from drop down to make it faster

Added duplicate check flow popup in submission also
</commit_message>
<xml_diff>
--- a/Mendix/input/data/Global_Material_Data.xlsx
+++ b/Mendix/input/data/Global_Material_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SatishKumarSundaramo\git\Mendix_New\Mendix\input\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E541DB-B184-467F-9E07-D15C5307B21A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046E1194-F6E5-4D25-8B96-8C98E8BF64BE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{92753D1E-95E7-49CB-AD96-B588CC3DB29F}"/>
   </bookViews>
@@ -408,9 +408,6 @@
     <t>Costing Method - Sales</t>
   </si>
   <si>
-    <t>KH001OC</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 
 Malt Pale C6 DE Koblenz </t>
   </si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>25000</t>
+  </si>
+  <si>
+    <t>SG001OC</t>
   </si>
 </sst>
 </file>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1D1E45-5652-489D-98CC-1DC9815FE9A3}">
   <dimension ref="A1:CC5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AM6" sqref="AM6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="5" spans="1:81" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>94</v>
@@ -1652,19 +1652,19 @@
         <v>76</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F5" s="4">
         <v>9</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>44</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J5" s="2">
         <v>1</v>
@@ -1673,7 +1673,7 @@
         <v>64</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M5" s="2" t="s">
         <v>41</v>
@@ -1694,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="T5" s="10" t="s">
         <v>46</v>
@@ -1703,7 +1703,7 @@
         <v>1</v>
       </c>
       <c r="V5" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="W5" s="10" t="s">
         <v>64</v>
@@ -1730,7 +1730,7 @@
         <v>49</v>
       </c>
       <c r="AE5" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AF5" s="10" t="s">
         <v>64</v>
@@ -1751,10 +1751,10 @@
         <v>52</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="AM5" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AN5" s="7" t="s">
         <v>64</v>
@@ -1799,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="BB5" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="BC5" s="6">
         <v>4</v>
       </c>
       <c r="BD5" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="BE5" s="12" t="s">
         <v>39</v>
@@ -1814,7 +1814,7 @@
         <v>0</v>
       </c>
       <c r="BG5" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="BH5" s="13">
         <v>0</v>
@@ -1832,19 +1832,19 @@
         <v>51</v>
       </c>
       <c r="BM5" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BN5" s="13" t="s">
         <v>51</v>
       </c>
       <c r="BO5" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="BP5" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="BP5" s="13" t="s">
+      <c r="BQ5" s="13" t="s">
         <v>140</v>
-      </c>
-      <c r="BQ5" s="13" t="s">
-        <v>141</v>
       </c>
       <c r="BR5" s="13">
         <v>7</v>
@@ -1865,20 +1865,20 @@
         <v>7</v>
       </c>
       <c r="BX5" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="BY5" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="BZ5" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="BY5" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="BZ5" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="CA5" s="13"/>
       <c r="CB5" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="CC5" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>